<commit_message>
add four more steps
</commit_message>
<xml_diff>
--- a/CheckList.xlsx
+++ b/CheckList.xlsx
@@ -16,66 +16,69 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="27">
   <si>
     <t>OS</t>
   </si>
   <si>
-    <t>Windows-10</t>
+    <t>Windows-10-10.0.18362-SP0</t>
   </si>
   <si>
     <t>Browser name</t>
   </si>
   <si>
+    <t>msedge</t>
+  </si>
+  <si>
+    <t>chrome</t>
+  </si>
+  <si>
+    <t>firefox</t>
+  </si>
+  <si>
+    <t>internet explorer</t>
+  </si>
+  <si>
     <t>opera</t>
   </si>
   <si>
-    <t>chrome</t>
-  </si>
-  <si>
-    <t>msedge</t>
-  </si>
-  <si>
-    <t>firefox</t>
-  </si>
-  <si>
-    <t>internet explorer</t>
-  </si>
-  <si>
     <t>Browser version</t>
   </si>
   <si>
+    <t>81.0.416.72</t>
+  </si>
+  <si>
+    <t>81.0.4044.138</t>
+  </si>
+  <si>
+    <t>75.0</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
     <t>81.0.4044.129</t>
   </si>
   <si>
-    <t>81.0.4044.138</t>
-  </si>
-  <si>
-    <t>81.0.416.72</t>
-  </si>
-  <si>
-    <t>75.0</t>
-  </si>
-  <si>
-    <t>11</t>
-  </si>
-  <si>
     <t>Last checked</t>
   </si>
   <si>
-    <t>09.05.2020_16.44.16</t>
-  </si>
-  <si>
-    <t>09.05.2020_16.47.04</t>
-  </si>
-  <si>
-    <t>09.05.2020_16.48.44</t>
-  </si>
-  <si>
-    <t>09.05.2020_16.52.08</t>
-  </si>
-  <si>
-    <t>09.05.2020_16.55.05</t>
+    <t>10.05.2020_13.50.05</t>
+  </si>
+  <si>
+    <t>10.05.2020_13.50.46</t>
+  </si>
+  <si>
+    <t>10.05.2020_13.51.29</t>
+  </si>
+  <si>
+    <t>10.05.2020_13.56.33</t>
+  </si>
+  <si>
+    <t>10.05.2020_13.57.41</t>
+  </si>
+  <si>
+    <t>10.05.2020_13.59.12</t>
   </si>
   <si>
     <t>Open Main page</t>
@@ -433,21 +436,16 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="29.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="19.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="22.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="20.140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="20.28515625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="19.85546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="18" style="1" customWidth="1"/>
+    <col min="2" max="7" width="26.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -463,11 +461,14 @@
       <c r="E1" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="G1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -484,10 +485,13 @@
         <v>6</v>
       </c>
       <c r="F2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:7">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -504,10 +508,13 @@
         <v>12</v>
       </c>
       <c r="F3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:7">
       <c r="A4" s="2" t="s">
         <v>14</v>
       </c>
@@ -526,45 +533,123 @@
       <c r="F4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="6" spans="1:6">
+      <c r="G4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
+        <v>22</v>
+      </c>
+      <c r="G6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
+        <v>23</v>
+      </c>
+      <c r="B7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" t="s">
+        <v>22</v>
+      </c>
+      <c r="G7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
+        <v>24</v>
+      </c>
+      <c r="B8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
+        <v>25</v>
+      </c>
+      <c r="B9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" t="s">
+        <v>22</v>
+      </c>
+      <c r="G9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
       <c r="A10" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
+      </c>
+      <c r="B10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10" t="s">
+        <v>22</v>
+      </c>
+      <c r="G10" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>